<commit_message>
Added files for using TangNano1K.
</commit_message>
<xml_diff>
--- a/MGSPICO2-xxx/partslist_MGSPICO2-02A.xlsx
+++ b/MGSPICO2-xxx/partslist_MGSPICO2-02A.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E166094-F6C3-4F6E-9FB6-5EE694CA436F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CB5158-3640-4C4B-AE2A-7861AE5CC263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2460" windowWidth="29235" windowHeight="16875" tabRatio="285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4965" yWindow="705" windowWidth="29340" windowHeight="19785" tabRatio="285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MGSPICO2-xxx" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="181">
   <si>
     <t>#</t>
   </si>
@@ -42,54 +42,33 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>C1, C6</t>
   </si>
   <si>
     <t>1500pF</t>
   </si>
   <si>
-    <t>0_Footprint:C_Rect_L6.5mm_W3.5mm_P3.50mm</t>
-  </si>
-  <si>
     <t>C2, C3, C4, C10, C11, C17</t>
   </si>
   <si>
-    <t>Capacitor_THT:CP_Radial_D5.0mm_P2.50mm</t>
-  </si>
-  <si>
     <t>C5, C14, C26</t>
   </si>
   <si>
     <t>C7, C9</t>
   </si>
   <si>
-    <t>SamacSys_Parts:CAPPRD250W50D630H600</t>
-  </si>
-  <si>
     <t>C8, C16, C19, C23</t>
   </si>
   <si>
-    <t>Capacitor_SMD:C_1206_3216Metric_Pad1.33x1.80mm_HandSolder</t>
-  </si>
-  <si>
     <t>C12, C13, C15, C18, C20</t>
   </si>
   <si>
     <t>1000pF</t>
   </si>
   <si>
-    <t>0_Footprint:C_Rect_L4.5mm_W3.5mm_P2.54mm</t>
-  </si>
-  <si>
     <t>C21</t>
   </si>
   <si>
-    <t>Capacitor_THT:CP_Radial_D8.0mm_P3.50mm</t>
-  </si>
-  <si>
     <t>C22, C24, C25</t>
   </si>
   <si>
@@ -102,15 +81,9 @@
     <t>MountingHole</t>
   </si>
   <si>
-    <t>MountingHole:MountingHole_3.2mm_M3</t>
-  </si>
-  <si>
     <t>IC1</t>
   </si>
   <si>
-    <t>Package_DIP:DIP-18_W7.62mm_Socket_LongPads</t>
-  </si>
-  <si>
     <t>IC2</t>
   </si>
   <si>
@@ -120,69 +93,45 @@
     <t>MJ-179PH(Center+)</t>
   </si>
   <si>
-    <t>0_Footprint:MJ179PH_N</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
     <t>AudioJack3</t>
   </si>
   <si>
-    <t>Connector_Audio:Jack_3.5mm_Switronic_ST-005-G_horizontal</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
     <t>Conn_01x01</t>
   </si>
   <si>
-    <t>Connector_PinHeader_2.54mm:PinHeader_1x01_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t>JP1, JP2, JP3, JP4, JP5</t>
   </si>
   <si>
     <t>Jumper</t>
   </si>
   <si>
-    <t>Connector_PinHeader_2.54mm:PinHeader_1x02_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t>JP6, JP7, JP8, JP9, JP10, JP11, JP12, JP13, JP14, JP15, JP16, JP17, JP18, JP19</t>
   </si>
   <si>
     <t>SolderJumper_2_Open</t>
   </si>
   <si>
-    <t>Jumper:SolderJumper-2_P1.3mm_Open_Pad1.0x1.5mm</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
-    <t>Inductor_THT:L_Radial_D7.8mm_P5.00mm_Fastron_07HCP</t>
-  </si>
-  <si>
     <t>PS1</t>
   </si>
   <si>
     <t>MCW03-05S05</t>
   </si>
   <si>
-    <t>MCW0305S05</t>
-  </si>
-  <si>
     <t>R1, R3, R14</t>
   </si>
   <si>
     <t>2.2K</t>
   </si>
   <si>
-    <t>Resistor_THT:R_Axial_DIN0207_L6.3mm_D2.5mm_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t>R2, R19, R37, R38, R39, R40, R41, R42, R43, R44, R45, R46</t>
   </si>
   <si>
@@ -213,9 +162,6 @@
     <t>R24</t>
   </si>
   <si>
-    <t>Resistor_SMD:R_1206_3216Metric_Pad1.30x1.75mm_HandSolder</t>
-  </si>
-  <si>
     <t>R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R36</t>
   </si>
   <si>
@@ -231,9 +177,6 @@
     <t>TVDP01-G73BB</t>
   </si>
   <si>
-    <t>TVDP01G73BB</t>
-  </si>
-  <si>
     <t>S4</t>
   </si>
   <si>
@@ -246,52 +189,31 @@
     <t>AE-Si5351A-B</t>
   </si>
   <si>
-    <t>0_Footprint:AE-Si5351A-B_DIP-8_300</t>
-  </si>
-  <si>
     <t>U2, U3, U4</t>
   </si>
   <si>
     <t>NJM4580</t>
   </si>
   <si>
-    <t>Package_DIP:DIP-8_W7.62mm_Socket_LongPads</t>
-  </si>
-  <si>
     <t>U5</t>
   </si>
   <si>
     <t>Pico</t>
   </si>
   <si>
-    <t>RPi_Pico:RPi_Pico_SMD_TH</t>
-  </si>
-  <si>
     <t>U6</t>
   </si>
   <si>
-    <t>TangNano</t>
-  </si>
-  <si>
-    <t>0_Footprint:TangNano_DIP-40_700</t>
-  </si>
-  <si>
     <t>U7</t>
   </si>
   <si>
     <t>OLED 128x64</t>
   </si>
   <si>
-    <t>0_Footprint:OLED Display I2C</t>
-  </si>
-  <si>
     <t>U8</t>
   </si>
   <si>
     <t>~</t>
-  </si>
-  <si>
-    <t>0_Footprint:Micro SD Card Socket</t>
   </si>
   <si>
     <t>VR1, VR2, VR3, VR4</t>
@@ -610,10 +532,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>02A</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>3362P-1-103LF</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -659,13 +577,6 @@
   </si>
   <si>
     <t>(販売終了)</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>代替品</t>
-    <rPh sb="0" eb="3">
-      <t>ダイタイヒン</t>
-    </rPh>
     <phoneticPr fontId="18"/>
   </si>
   <si>
@@ -743,6 +654,78 @@
   </si>
   <si>
     <t>https://eleshop.jp/shop/g/gD1V412/</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TangNano 1K</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TangNano</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TangNano1K</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>https://wiki.sipeed.com/hardware/en/tang/Tang-Nano-1K/Nano-1k.html</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>https://wiki.sipeed.com/hardware/en/tang/Tang-Nano/Nano.html</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>YMZ294-D</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>YMZ284-D</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>※取り付け位置に注意です。1</t>
+    <rPh sb="1" eb="2">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ツ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>MGSPICO2-02A</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>代替品(Replacement)</t>
+    <rPh sb="0" eb="3">
+      <t>ダイタイヒン</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TangNano (GW1N-1)  ※mmmscc.fs</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TangNano1K (GW1NZ-LV1) ※mmmscc_tn1k.fs   ※回路に修正が必要です</t>
+    <rPh sb="42" eb="44">
+      <t>カイロ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>シュウセイ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ヒツヨウ</t>
+    </rPh>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1404,7 +1387,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1450,21 +1433,15 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1475,6 +1452,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1853,10 +1833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1864,19 +1844,22 @@
     <col min="2" max="2" width="29.875" customWidth="1"/>
     <col min="3" max="3" width="4.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="76.5" customWidth="1"/>
-    <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" customWidth="1"/>
-    <col min="10" max="10" width="57.75" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="76.5" customWidth="1"/>
+    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" customWidth="1"/>
+    <col min="9" max="9" width="57.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+        <v>177</v>
+      </c>
+      <c r="I1" s="22">
+        <v>45499</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1889,144 +1872,129 @@
       <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>6</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <v>3</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I5" s="2">
+        <v>75</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="2">
         <v>117877</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="I5" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+        <v>78</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -2034,89 +2002,80 @@
       <c r="D7" s="10">
         <v>104</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="E7" s="6"/>
+      <c r="F7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="2">
         <v>115180</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="I7" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2">
         <v>5</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2">
         <v>3</v>
@@ -2124,29 +2083,26 @@
       <c r="D10" s="10">
         <v>106</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I10" s="2">
+      <c r="E10" s="6"/>
+      <c r="F10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="2">
         <v>103095</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="I10" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -2154,439 +2110,391 @@
       <c r="D11" s="10">
         <v>103</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="2">
+      <c r="E11" s="6"/>
+      <c r="F11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="2">
         <v>104063</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A12" s="20">
+      <c r="I11" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12" s="18">
         <v>10</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="20">
+      <c r="B12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="18">
         <v>4</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="D12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>150</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="18"/>
-      <c r="K13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="17"/>
+      <c r="J13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" s="15">
+        <v>148</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="4">
         <v>112141</v>
       </c>
-      <c r="J14" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="K14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="I14" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="J14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="2">
+        <v>20</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="2">
         <v>106568</v>
       </c>
-      <c r="J15" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="I15" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I16" s="2">
+        <v>22</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="2">
         <v>102460</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I16" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C18" s="2">
         <v>5</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2">
         <v>14</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I21" s="2">
+        <v>31</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="2">
         <v>104261</v>
       </c>
-      <c r="J21" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I21" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2">
         <v>3</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>132</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2">
         <v>12</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I23" s="2">
+        <v>35</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="2">
         <v>108535</v>
       </c>
-      <c r="J23" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I23" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="2">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2">
         <v>7</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2">
+        <v>37</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2">
         <v>116640</v>
       </c>
-      <c r="J24" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I24" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2">
         <v>8</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>188</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="2">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C26" s="2">
         <v>2</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>189</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="2">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
@@ -2594,85 +2502,76 @@
       <c r="D27" s="10">
         <v>47</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>190</v>
-      </c>
+      <c r="E27" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="2">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C28" s="2">
         <v>1</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="2">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C29" s="2">
         <v>12</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I29" s="2">
+        <v>45</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="2">
         <v>108539</v>
       </c>
-      <c r="J29" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I29" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="2">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -2680,494 +2579,508 @@
       <c r="D30" s="10">
         <v>470</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="E30" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="2">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C31" s="2">
         <v>3</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I31" s="2">
+        <v>48</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="2">
         <v>109824</v>
       </c>
-      <c r="J31" s="11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I31" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="2">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I32" s="2">
+        <v>50</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="2">
         <v>115707</v>
       </c>
-      <c r="J32" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I32" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="2">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I33" s="5">
+      <c r="H33" s="5">
         <v>110679</v>
       </c>
-      <c r="J33" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I33" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="2">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C34" s="2">
         <v>3</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I34" s="5">
+        <v>54</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34" s="5">
         <v>100069</v>
       </c>
-      <c r="J34" s="11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I34" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="2">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I35" s="2">
+        <v>56</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H35" s="2">
         <v>116132</v>
       </c>
-      <c r="J35" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I35" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="2">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>117</v>
+        <v>170</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="2">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I37" s="2">
+        <v>59</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H37" s="2">
         <v>112031</v>
       </c>
-      <c r="J37" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I37" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="2">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C38" s="2">
         <v>1</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F38" s="6"/>
-      <c r="G38" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+        <v>61</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H38" s="2"/>
+      <c r="I38" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="2">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C39" s="2">
         <v>4</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I39" s="5">
+        <v>63</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" s="5">
         <v>114905</v>
       </c>
-      <c r="J39" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="J40" s="12"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I39" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="J41" s="12"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+        <v>178</v>
+      </c>
+      <c r="I41" s="12"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="2">
         <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C42" s="2">
         <v>6</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="I42" s="2"/>
-      <c r="J42" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H42" s="2"/>
+      <c r="I42" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="2">
+        <v>12</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G43" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="11"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A44" s="2">
+        <v>18</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="11" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A45" s="2">
+        <v>34</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+      <c r="D45" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="E45" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="I43" s="2"/>
-      <c r="J43" s="11" t="s">
+      <c r="F45" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A44" s="2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" s="2">
         <v>37</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="2">
+      <c r="B46" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="2">
         <v>4</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I44" s="2">
+      <c r="D46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H46" s="2">
         <v>103277</v>
       </c>
-      <c r="J44" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B45" s="12"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="J45" s="14"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A46" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2">
+      <c r="I46" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G47" s="12"/>
+      <c r="I47" s="14"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B48" s="12"/>
+      <c r="D48" s="13"/>
+      <c r="G48" s="12"/>
+      <c r="I48" s="14"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A49" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2">
         <v>3</v>
       </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I47" s="2">
+      <c r="D50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H50" s="2">
         <v>100035</v>
       </c>
-      <c r="J47" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2">
+      <c r="I50" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2">
         <v>2</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I48" s="2">
+      <c r="D51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H51" s="2">
         <v>100030</v>
       </c>
-      <c r="J48" s="3" t="s">
-        <v>186</v>
+      <c r="I51" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P39">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O39">
     <sortCondition ref="A3:A39"/>
   </sortState>
   <phoneticPr fontId="18"/>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="J4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="J5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="J6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="J7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="J8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="J9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="J10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="J11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="J15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="J16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="J20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="J21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="J28" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="J29" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="J23" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="J31" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="J32" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="J33" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="J34" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="J39" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="J35" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="J37" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="J43" r:id="rId24" xr:uid="{7C9F06ED-5A8D-45E7-8720-14E95F889B06}"/>
-    <hyperlink ref="J44" r:id="rId25" xr:uid="{3CDAF813-227B-4677-8CC0-D87C2EB5DB04}"/>
-    <hyperlink ref="J14" r:id="rId26" xr:uid="{AD62D4D0-BC76-4F3C-8AF9-54AB50A0F785}"/>
-    <hyperlink ref="J47" r:id="rId27" xr:uid="{7DD5DC37-997B-40EA-9686-22742B1BECBF}"/>
-    <hyperlink ref="J48" r:id="rId28" xr:uid="{E12C1B07-193A-4D98-B075-A4AB6A55A843}"/>
-    <hyperlink ref="J24" r:id="rId29" xr:uid="{90D37F50-8315-4F7A-BB4A-432240493846}"/>
-    <hyperlink ref="J42" r:id="rId30" xr:uid="{71EE1E27-8968-4A9F-8EBE-381C1633F805}"/>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="I15" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="I20" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="I21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="I28" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="I29" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="I23" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="I31" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="I32" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="I33" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="I34" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="I39" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="I35" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="I37" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="I44" r:id="rId24" xr:uid="{7C9F06ED-5A8D-45E7-8720-14E95F889B06}"/>
+    <hyperlink ref="I46" r:id="rId25" xr:uid="{3CDAF813-227B-4677-8CC0-D87C2EB5DB04}"/>
+    <hyperlink ref="I14" r:id="rId26" xr:uid="{AD62D4D0-BC76-4F3C-8AF9-54AB50A0F785}"/>
+    <hyperlink ref="I50" r:id="rId27" xr:uid="{7DD5DC37-997B-40EA-9686-22742B1BECBF}"/>
+    <hyperlink ref="I51" r:id="rId28" xr:uid="{E12C1B07-193A-4D98-B075-A4AB6A55A843}"/>
+    <hyperlink ref="I24" r:id="rId29" xr:uid="{90D37F50-8315-4F7A-BB4A-432240493846}"/>
+    <hyperlink ref="I42" r:id="rId30" xr:uid="{71EE1E27-8968-4A9F-8EBE-381C1633F805}"/>
+    <hyperlink ref="I36" r:id="rId31" xr:uid="{7D6050BF-C4E6-46CA-BD12-1F97D4372E46}"/>
+    <hyperlink ref="I45" r:id="rId32" xr:uid="{1785AD6F-2244-43B8-94FD-B3D5CDCA8BA7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>